<commit_message>
updating with latest user list (Dec)
</commit_message>
<xml_diff>
--- a/group-accounts/ebd_users_GA_relDec-2021.xlsx
+++ b/group-accounts/ebd_users_GA_relDec-2021.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="908" uniqueCount="880">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="907" uniqueCount="879">
   <si>
     <t xml:space="preserve">OBSERVER.ID</t>
   </si>
@@ -2456,15 +2456,6 @@
     <t xml:space="preserve">Birds of Bellezea</t>
   </si>
   <si>
-    <t xml:space="preserve">obsr826579</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Single observer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KalaiSelvan V</t>
-  </si>
-  <si>
     <t xml:space="preserve">obsr2809001</t>
   </si>
   <si>
@@ -2505,6 +2496,12 @@
   </si>
   <si>
     <t xml:space="preserve">Bird Nerd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">obsr2607928</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patch Monitoring India</t>
   </si>
   <si>
     <t xml:space="preserve">obsr2601832</t>
@@ -2770,8 +2767,8 @@
   </sheetPr>
   <dimension ref="A1:E428"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C428" activeCellId="0" sqref="C428"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A397" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D408" activeCellId="0" sqref="D408"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8486,88 +8483,88 @@
         <v>0</v>
       </c>
       <c r="C401" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D401" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E401" s="0" t="s">
         <v>812</v>
-      </c>
-      <c r="E401" s="0" t="s">
-        <v>813</v>
       </c>
     </row>
     <row r="402" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A402" s="0" t="s">
+        <v>813</v>
+      </c>
+      <c r="B402" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C402" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E402" s="0" t="s">
         <v>814</v>
-      </c>
-      <c r="B402" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C402" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E402" s="0" t="s">
-        <v>815</v>
       </c>
     </row>
     <row r="403" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A403" s="0" t="s">
+        <v>815</v>
+      </c>
+      <c r="B403" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C403" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E403" s="0" t="s">
         <v>816</v>
-      </c>
-      <c r="B403" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C403" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E403" s="0" t="s">
-        <v>817</v>
       </c>
     </row>
     <row r="404" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A404" s="0" t="s">
+        <v>817</v>
+      </c>
+      <c r="B404" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C404" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E404" s="0" t="s">
         <v>818</v>
-      </c>
-      <c r="B404" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C404" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E404" s="0" t="s">
-        <v>819</v>
       </c>
     </row>
     <row r="405" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A405" s="0" t="s">
+        <v>819</v>
+      </c>
+      <c r="B405" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C405" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E405" s="0" t="s">
         <v>820</v>
-      </c>
-      <c r="B405" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C405" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E405" s="0" t="s">
-        <v>821</v>
       </c>
     </row>
     <row r="406" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A406" s="0" t="s">
+        <v>821</v>
+      </c>
+      <c r="B406" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C406" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D406" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="E406" s="0" t="s">
         <v>822</v>
-      </c>
-      <c r="B406" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C406" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E406" s="0" t="s">
-        <v>823</v>
       </c>
     </row>
     <row r="407" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A407" s="0" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B407" s="0" t="n">
         <v>0</v>
@@ -8579,57 +8576,54 @@
         <v>131</v>
       </c>
       <c r="E407" s="0" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
     </row>
     <row r="408" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A408" s="0" t="s">
+        <v>825</v>
+      </c>
+      <c r="B408" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C408" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E408" s="0" t="s">
         <v>826</v>
-      </c>
-      <c r="B408" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C408" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D408" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="E408" s="0" t="s">
-        <v>827</v>
       </c>
     </row>
     <row r="409" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A409" s="0" t="s">
+        <v>827</v>
+      </c>
+      <c r="B409" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C409" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E409" s="0" t="s">
         <v>828</v>
-      </c>
-      <c r="B409" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C409" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E409" s="0" t="s">
-        <v>829</v>
       </c>
     </row>
     <row r="410" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A410" s="0" t="s">
+        <v>829</v>
+      </c>
+      <c r="B410" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C410" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E410" s="0" t="s">
         <v>830</v>
-      </c>
-      <c r="B410" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C410" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E410" s="0" t="s">
-        <v>831</v>
       </c>
     </row>
     <row r="411" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A411" s="0" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="B411" s="0" t="n">
         <v>0</v>
@@ -8641,110 +8635,110 @@
         <v>131</v>
       </c>
       <c r="E411" s="0" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="412" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A412" s="0" t="s">
+        <v>833</v>
+      </c>
+      <c r="B412" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C412" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E412" s="0" t="s">
         <v>834</v>
-      </c>
-      <c r="B412" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C412" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E412" s="0" t="s">
-        <v>835</v>
       </c>
     </row>
     <row r="413" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A413" s="0" t="s">
+        <v>835</v>
+      </c>
+      <c r="B413" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C413" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E413" s="0" t="s">
         <v>836</v>
-      </c>
-      <c r="B413" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C413" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E413" s="0" t="s">
-        <v>837</v>
       </c>
     </row>
     <row r="414" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A414" s="0" t="s">
+        <v>837</v>
+      </c>
+      <c r="B414" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C414" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E414" s="0" t="s">
         <v>838</v>
-      </c>
-      <c r="B414" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C414" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E414" s="0" t="s">
-        <v>839</v>
       </c>
     </row>
     <row r="415" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A415" s="0" t="s">
+        <v>839</v>
+      </c>
+      <c r="B415" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C415" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E415" s="0" t="s">
         <v>840</v>
-      </c>
-      <c r="B415" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C415" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E415" s="0" t="s">
-        <v>841</v>
       </c>
     </row>
     <row r="416" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A416" s="0" t="s">
+        <v>841</v>
+      </c>
+      <c r="B416" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C416" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E416" s="0" t="s">
         <v>842</v>
-      </c>
-      <c r="B416" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C416" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E416" s="0" t="s">
-        <v>843</v>
       </c>
     </row>
     <row r="417" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A417" s="0" t="s">
+        <v>843</v>
+      </c>
+      <c r="B417" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C417" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E417" s="0" t="s">
         <v>844</v>
-      </c>
-      <c r="B417" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C417" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E417" s="0" t="s">
-        <v>845</v>
       </c>
     </row>
     <row r="418" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A418" s="0" t="s">
+        <v>845</v>
+      </c>
+      <c r="B418" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C418" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E418" s="0" t="s">
         <v>846</v>
-      </c>
-      <c r="B418" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C418" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E418" s="0" t="s">
-        <v>847</v>
       </c>
     </row>
     <row r="419" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A419" s="0" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="B419" s="0" t="n">
         <v>0</v>
@@ -8756,96 +8750,96 @@
         <v>131</v>
       </c>
       <c r="E419" s="0" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="420" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A420" s="0" t="s">
+        <v>849</v>
+      </c>
+      <c r="B420" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C420" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E420" s="0" t="s">
         <v>850</v>
-      </c>
-      <c r="B420" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C420" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E420" s="0" t="s">
-        <v>851</v>
       </c>
     </row>
     <row r="421" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A421" s="0" t="s">
+        <v>851</v>
+      </c>
+      <c r="B421" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C421" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E421" s="0" t="s">
         <v>852</v>
-      </c>
-      <c r="B421" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C421" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E421" s="0" t="s">
-        <v>853</v>
       </c>
     </row>
     <row r="422" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A422" s="0" t="s">
+        <v>853</v>
+      </c>
+      <c r="B422" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C422" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E422" s="0" t="s">
         <v>854</v>
-      </c>
-      <c r="B422" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C422" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E422" s="0" t="s">
-        <v>855</v>
       </c>
     </row>
     <row r="423" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A423" s="0" t="s">
+        <v>855</v>
+      </c>
+      <c r="B423" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C423" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E423" s="0" t="s">
         <v>856</v>
-      </c>
-      <c r="B423" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C423" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E423" s="0" t="s">
-        <v>857</v>
       </c>
     </row>
     <row r="424" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A424" s="0" t="s">
+        <v>857</v>
+      </c>
+      <c r="B424" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C424" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E424" s="0" t="s">
         <v>858</v>
-      </c>
-      <c r="B424" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C424" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E424" s="0" t="s">
-        <v>859</v>
       </c>
     </row>
     <row r="425" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A425" s="0" t="s">
+        <v>859</v>
+      </c>
+      <c r="B425" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C425" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E425" s="0" t="s">
         <v>860</v>
-      </c>
-      <c r="B425" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C425" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E425" s="0" t="s">
-        <v>861</v>
       </c>
     </row>
     <row r="426" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A426" s="0" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="B426" s="0" t="n">
         <v>0</v>
@@ -8857,35 +8851,35 @@
         <v>131</v>
       </c>
       <c r="E426" s="0" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
     </row>
     <row r="427" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A427" s="0" t="s">
+        <v>863</v>
+      </c>
+      <c r="B427" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C427" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E427" s="0" t="s">
         <v>864</v>
-      </c>
-      <c r="B427" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C427" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E427" s="0" t="s">
-        <v>865</v>
       </c>
     </row>
     <row r="428" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A428" s="0" t="s">
+        <v>865</v>
+      </c>
+      <c r="B428" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C428" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E428" s="0" t="s">
         <v>866</v>
-      </c>
-      <c r="B428" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C428" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E428" s="0" t="s">
-        <v>867</v>
       </c>
     </row>
   </sheetData>
@@ -8907,32 +8901,32 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.53515625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.89"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8940,7 +8934,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8948,37 +8942,37 @@
         <v>2</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
     </row>
   </sheetData>

</xml_diff>